<commit_message>
update data test I don't know
</commit_message>
<xml_diff>
--- a/config/Scope.xlsx
+++ b/config/Scope.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tool_test_game\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16384D46-FB1F-473B-8BB6-A902EDC465D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DE08DC-0933-4D8E-A81E-0B15D631CAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Level</t>
   </si>
@@ -106,11 +106,15 @@
   <si>
     <t>FILE:report\list_fail.txt</t>
   </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -27474,15 +27478,15 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.140625"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125"/>
+    <col min="11" max="11" customWidth="true" width="24.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -27531,22 +27535,22 @@
         <v>27</v>
       </c>
       <c r="D2" s="7">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E2" s="7">
-        <v>27</v>
+        <v>16</v>
       </c>
-      <c r="F2">
-        <v>4</v>
+      <c r="F2" s="0" t="n">
+        <v>16.0</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="8">
-        <v>4</v>
+      <c r="I2" s="8" t="n">
+        <v>4.0</v>
       </c>
-      <c r="J2" s="8">
-        <v>0</v>
+      <c r="J2" s="8" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -27587,7 +27591,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="45.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1">
@@ -27635,7 +27639,7 @@
       <c r="C2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>16</v>
       </c>
       <c r="E2" s="12"/>

</xml_diff>

<commit_message>
update file data file jar
</commit_message>
<xml_diff>
--- a/config/Scope.xlsx
+++ b/config/Scope.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tool_test_game\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F39D308-63DB-497A-AFB9-DD2A473648C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5BA46E-1A38-4806-ADC7-72F1B154E527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Level</t>
   </si>
@@ -104,13 +104,17 @@
     <t>$.topic_name,$.part</t>
   </si>
   <si>
-    <t>FILE:report\list_fail.txt</t>
+    <t>FILE::report\list_fail.txt</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -27474,15 +27478,15 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.140625"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125"/>
+    <col min="11" max="11" customWidth="true" width="24.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -27528,25 +27532,25 @@
         <v>7</v>
       </c>
       <c r="C2" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
       </c>
       <c r="E2" s="7">
-        <v>27</v>
+        <v>30</v>
       </c>
-      <c r="F2">
-        <v>3</v>
+      <c r="F2" s="0" t="n">
+        <v>11.0</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="8">
-        <v>3</v>
+      <c r="I2" s="8" t="n">
+        <v>0.0</v>
       </c>
-      <c r="J2" s="8">
-        <v>0</v>
+      <c r="J2" s="8" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -27587,7 +27591,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="45.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1">
@@ -27635,8 +27639,8 @@
       <c r="C2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
+      <c r="D2" t="s" s="0">
+        <v>26</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10"/>

</xml_diff>

<commit_message>
update tec monkey go letterfishing
</commit_message>
<xml_diff>
--- a/config/Scope.xlsx
+++ b/config/Scope.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tool_test_game\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="375" yWindow="795" windowWidth="21600" windowHeight="11385" activeTab="5"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Scope" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Plan" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Options" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Group-Turn" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Note" sheetId="5" r:id="rId8"/>
+    <sheet name="Scope" sheetId="1" r:id="rId3"/>
+    <sheet name="Plan" sheetId="2" r:id="rId4"/>
+    <sheet name="Options" sheetId="3" r:id="rId5"/>
+    <sheet name="Group-Turn" sheetId="4" r:id="rId6"/>
+    <sheet name="Note" sheetId="5" r:id="rId7"/>
+    <sheet name="Evaluation Warning" sheetId="7" r:id="rId8"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="Wqrab3t6a9P+8657acRiy3PPnRgyPXlHeqJS7A1TITw="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>STT</t>
   </si>
@@ -40,22 +44,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Report_Play lesson</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Report_GameName</t>
-  </si>
-  <si>
-    <t>G_act</t>
   </si>
   <si>
     <t>FLow</t>
@@ -85,7 +77,10 @@
     <t>Course</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
   <si>
     <t>FILE::report\list_fail.txt</t>
@@ -97,16 +92,10 @@
     <t>$.level</t>
   </si>
   <si>
-    <t>$.lesson</t>
-  </si>
-  <si>
     <t>$.topic</t>
   </si>
   <si>
     <t>AI_Speak</t>
-  </si>
-  <si>
-    <t>app</t>
   </si>
   <si>
     <t>Flow</t>
@@ -122,9 +111,6 @@
   </si>
   <si>
     <t>EE</t>
-  </si>
-  <si>
-    <t>api</t>
   </si>
   <si>
     <t>Advanced</t>
@@ -148,210 +134,325 @@
     <t>Description</t>
   </si>
   <si>
-    <t>$.act.length()</t>
-  </si>
-  <si>
-    <t>Tổng số act</t>
-  </si>
-  <si>
     <t>Xác định end game sau mỗi testcase hay chuyển act</t>
   </si>
   <si>
     <t>Xác định thêm end game sẽ phân biệt dễ hơn chuyển act hay end game</t>
   </si>
+  <si>
+    <t>$.name</t>
+  </si>
+  <si>
+    <t>$.act_id</t>
+  </si>
+  <si>
+    <t>M_go</t>
+  </si>
+  <si>
+    <t>Report_GS01LetterFishing(Clone)</t>
+  </si>
+  <si>
+    <t>Report_Play game</t>
+  </si>
+  <si>
+    <t>Evaluation Only. Created with Aspose.Cells for Java.Copyright 2003 - 2021 Aspose Pty Ltd.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="9">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="13.0"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="&quot;Times New Roman&quot;"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D2E9"/>
-        <bgColor rgb="FFD9D2E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD2F1DA"/>
-        <bgColor rgb="FFD2F1DA"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF9FC5E8"/>
           <bgColor rgb="FF9FC5E8"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -541,28 +642,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection activeCell="D2" sqref="D2" pane="topRight"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.88"/>
-    <col customWidth="1" min="2" max="2" width="45.75"/>
+    <col min="1" max="1" customWidth="true" width="5.857142857142857"/>
+    <col min="2" max="2" customWidth="true" width="45.714285714285715"/>
+    <col min="3" max="6" customWidth="true" width="12.571428571428571"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,18 +704,18 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="4"/>
@@ -634,141 +739,152 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="7">
+        <v>2.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="E5" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="D1:D5">
+    <cfRule type="cellIs" priority="1" dxfId="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D3">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" priority="2" dxfId="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D3">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" priority="3" dxfId="0" operator="equal">
       <formula>"SKIP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E3">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>'Group-Turn'!$A:$A</formula1>
     </dataValidation>
   </dataValidations>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.13"/>
-    <col customWidth="1" min="5" max="5" width="13.75"/>
-    <col customWidth="1" min="7" max="8" width="26.38"/>
-    <col customWidth="1" min="9" max="9" width="15.5"/>
-    <col customWidth="1" min="11" max="11" width="20.75"/>
-    <col customWidth="1" min="12" max="12" width="24.0"/>
+    <col min="1" max="1" customWidth="true" width="13.142857142857142"/>
+    <col min="2" max="4" customWidth="true" width="12.571428571428571"/>
+    <col min="5" max="5" customWidth="true" width="13.714285714285714"/>
+    <col min="6" max="6" customWidth="true" width="12.571428571428571"/>
+    <col min="7" max="8" customWidth="true" width="26.428571428571427"/>
+    <col min="9" max="9" customWidth="true" width="15.428571428571429"/>
+    <col min="12" max="12" customWidth="true" width="24.0"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.0" customHeight="1">
+    <row r="1" spans="1:12" ht="15" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="L1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="16.5">
+      <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="B2" s="12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="13">
-        <v>30.0</v>
+        <v>1.0</v>
       </c>
       <c r="D2" s="13">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="E2" s="13">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="F2" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="13" t="n">
         <v>0.0</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>25</v>
+      <c r="K2" s="13" t="n">
+        <v>0.0</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="13"/>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2">
-      <formula1>Options!$D$2:$D2</formula1>
-    </dataValidation>
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2">
       <formula1>Options!$C:$C</formula1>
     </dataValidation>
@@ -779,37 +895,38 @@
       <formula1>Options!$B$2:$B2</formula1>
     </dataValidation>
   </dataValidations>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="6" customWidth="true" width="12.571428571428571"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="15" t="s">
-        <v>13</v>
+    <row r="1" spans="1:25" ht="15" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>9</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>29</v>
+      <c r="B1" s="14" t="s">
+        <v>24</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>20</v>
+      <c r="C1" s="14" t="s">
+        <v>16</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>21</v>
-      </c>
+      <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
@@ -832,19 +949,17 @@
       <c r="X1" s="12"/>
       <c r="Y1" s="12"/>
     </row>
-    <row r="2" ht="15.0" customHeight="1">
+    <row r="2" spans="1:25" ht="15" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>28</v>
-      </c>
+      <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -867,19 +982,17 @@
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
     </row>
-    <row r="3" ht="15.0" customHeight="1">
+    <row r="3" spans="1:25" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
@@ -902,13 +1015,13 @@
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
     </row>
-    <row r="4" ht="15.0" customHeight="1">
+    <row r="4" spans="1:25" ht="15" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -933,12 +1046,14 @@
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
     </row>
-    <row r="5" ht="15.0" customHeight="1">
+    <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -962,9 +1077,9 @@
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
     </row>
-    <row r="6" ht="15.0" customHeight="1">
+    <row r="6" spans="1:25" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -991,9 +1106,9 @@
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
     </row>
-    <row r="7" ht="15.0" customHeight="1">
-      <c r="A7" s="18" t="s">
-        <v>24</v>
+    <row r="7" spans="1:25" ht="15" customHeight="1">
+      <c r="A7" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -1020,9 +1135,9 @@
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" ht="15.0" customHeight="1">
+    <row r="8" spans="1:25" ht="15" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -1049,8 +1164,10 @@
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" ht="15.0" customHeight="1">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:25" ht="15" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1076,7 +1193,7 @@
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
     </row>
-    <row r="10" ht="15.0" customHeight="1">
+    <row r="10" spans="1:25" ht="15" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -1103,7 +1220,7 @@
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" ht="15.0" customHeight="1">
+    <row r="11" spans="1:25" ht="15" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -1130,7 +1247,7 @@
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
     </row>
-    <row r="12" ht="15.0" customHeight="1">
+    <row r="12" spans="1:25" ht="15" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1157,7 +1274,7 @@
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
     </row>
-    <row r="13" ht="15.0" customHeight="1">
+    <row r="13" spans="1:25" ht="15" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -1184,7 +1301,7 @@
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
     </row>
-    <row r="14" ht="15.0" customHeight="1">
+    <row r="14" spans="1:25" ht="15" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -1211,7 +1328,7 @@
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
     </row>
-    <row r="15" ht="15.0" customHeight="1">
+    <row r="15" spans="1:25" ht="15" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1238,7 +1355,7 @@
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
     </row>
-    <row r="16" ht="15.0" customHeight="1">
+    <row r="16" spans="1:25" ht="15" customHeight="1">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -1265,7 +1382,7 @@
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
     </row>
-    <row r="17" ht="15.0" customHeight="1">
+    <row r="17" spans="1:25" ht="15" customHeight="1">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1292,7 +1409,7 @@
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" ht="15.0" customHeight="1">
+    <row r="18" spans="1:25" ht="15" customHeight="1">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1319,7 +1436,7 @@
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
     </row>
-    <row r="19" ht="15.0" customHeight="1">
+    <row r="19" spans="1:25" ht="15" customHeight="1">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1346,7 +1463,7 @@
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
     </row>
-    <row r="20" ht="15.0" customHeight="1">
+    <row r="20" spans="1:25" ht="15" customHeight="1">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1373,7 +1490,7 @@
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
     </row>
-    <row r="21" ht="15.0" customHeight="1">
+    <row r="21" spans="1:25" ht="15" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1400,7 +1517,7 @@
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
     </row>
-    <row r="22" ht="15.0" customHeight="1">
+    <row r="22" spans="1:25" ht="15" customHeight="1">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1427,7 +1544,7 @@
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
     </row>
-    <row r="23" ht="15.0" customHeight="1">
+    <row r="23" spans="1:25" ht="15" customHeight="1">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1454,7 +1571,7 @@
       <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
     </row>
-    <row r="24" ht="15.0" customHeight="1">
+    <row r="24" spans="1:25" ht="15" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -1481,7 +1598,7 @@
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
     </row>
-    <row r="25" ht="15.0" customHeight="1">
+    <row r="25" spans="1:25" ht="15" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -1508,7 +1625,7 @@
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
     </row>
-    <row r="26" ht="15.0" customHeight="1">
+    <row r="26" spans="1:25" ht="15" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -1535,7 +1652,7 @@
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
     </row>
-    <row r="27" ht="15.0" customHeight="1">
+    <row r="27" spans="1:25" ht="15" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1562,7 +1679,7 @@
       <c r="X27" s="12"/>
       <c r="Y27" s="12"/>
     </row>
-    <row r="28" ht="15.0" customHeight="1">
+    <row r="28" spans="1:25" ht="15" customHeight="1">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1589,7 +1706,7 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" ht="15.0" customHeight="1">
+    <row r="29" spans="1:25" ht="15" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1616,7 +1733,7 @@
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
     </row>
-    <row r="30" ht="15.0" customHeight="1">
+    <row r="30" spans="1:25" ht="15" customHeight="1">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1643,7 +1760,7 @@
       <c r="X30" s="12"/>
       <c r="Y30" s="12"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:25" ht="15.75" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1670,7 +1787,7 @@
       <c r="X31" s="12"/>
       <c r="Y31" s="12"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:25" ht="15.75" customHeight="1">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1697,7 +1814,7 @@
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:25" ht="15.75" customHeight="1">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1724,7 +1841,7 @@
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:25" ht="15.75" customHeight="1">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -1751,7 +1868,7 @@
       <c r="X34" s="12"/>
       <c r="Y34" s="12"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:25" ht="15.75" customHeight="1">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -1778,7 +1895,7 @@
       <c r="X35" s="12"/>
       <c r="Y35" s="12"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:25" ht="15.75" customHeight="1">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -1805,7 +1922,7 @@
       <c r="X36" s="12"/>
       <c r="Y36" s="12"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:25" ht="15.75" customHeight="1">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -1832,7 +1949,7 @@
       <c r="X37" s="12"/>
       <c r="Y37" s="12"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:25" ht="15.75" customHeight="1">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -1859,7 +1976,7 @@
       <c r="X38" s="12"/>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:25" ht="15.75" customHeight="1">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -1886,7 +2003,7 @@
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:25" ht="15.75" customHeight="1">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -1913,7 +2030,7 @@
       <c r="X40" s="12"/>
       <c r="Y40" s="12"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:25" ht="15.75" customHeight="1">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -1940,7 +2057,7 @@
       <c r="X41" s="12"/>
       <c r="Y41" s="12"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:25" ht="15.75" customHeight="1">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -1967,7 +2084,7 @@
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:25" ht="15.75" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -1994,7 +2111,7 @@
       <c r="X43" s="12"/>
       <c r="Y43" s="12"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:25" ht="15.75" customHeight="1">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -2021,7 +2138,7 @@
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:25" ht="15.75" customHeight="1">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -2048,7 +2165,7 @@
       <c r="X45" s="12"/>
       <c r="Y45" s="12"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:25" ht="15.75" customHeight="1">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -2075,7 +2192,7 @@
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -2102,7 +2219,7 @@
       <c r="X47" s="12"/>
       <c r="Y47" s="12"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:25" ht="15.75" customHeight="1">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -2129,7 +2246,7 @@
       <c r="X48" s="12"/>
       <c r="Y48" s="12"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:25" ht="15.75" customHeight="1">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -2156,7 +2273,7 @@
       <c r="X49" s="12"/>
       <c r="Y49" s="12"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:25" ht="15.75" customHeight="1">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -2183,7 +2300,7 @@
       <c r="X50" s="12"/>
       <c r="Y50" s="12"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:25" ht="15.75" customHeight="1">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -2210,7 +2327,7 @@
       <c r="X51" s="12"/>
       <c r="Y51" s="12"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:25" ht="15.75" customHeight="1">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -2237,7 +2354,7 @@
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:25" ht="15.75" customHeight="1">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -2264,7 +2381,7 @@
       <c r="X53" s="12"/>
       <c r="Y53" s="12"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" spans="1:25" ht="15.75" customHeight="1">
       <c r="A54" s="12"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
@@ -2291,7 +2408,7 @@
       <c r="X54" s="12"/>
       <c r="Y54" s="12"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="1:25" ht="15.75" customHeight="1">
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -2318,7 +2435,7 @@
       <c r="X55" s="12"/>
       <c r="Y55" s="12"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:25" ht="15.75" customHeight="1">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -2345,7 +2462,7 @@
       <c r="X56" s="12"/>
       <c r="Y56" s="12"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:25" ht="15.75" customHeight="1">
       <c r="A57" s="12"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
@@ -2372,7 +2489,7 @@
       <c r="X57" s="12"/>
       <c r="Y57" s="12"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:25" ht="15.75" customHeight="1">
       <c r="A58" s="12"/>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
@@ -2399,7 +2516,7 @@
       <c r="X58" s="12"/>
       <c r="Y58" s="12"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" spans="1:25" ht="15.75" customHeight="1">
       <c r="A59" s="12"/>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
@@ -2426,7 +2543,7 @@
       <c r="X59" s="12"/>
       <c r="Y59" s="12"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:25" ht="15.75" customHeight="1">
       <c r="A60" s="12"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
@@ -2453,7 +2570,7 @@
       <c r="X60" s="12"/>
       <c r="Y60" s="12"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:25" ht="15.75" customHeight="1">
       <c r="A61" s="12"/>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
@@ -2480,7 +2597,7 @@
       <c r="X61" s="12"/>
       <c r="Y61" s="12"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:25" ht="15.75" customHeight="1">
       <c r="A62" s="12"/>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
@@ -2507,7 +2624,7 @@
       <c r="X62" s="12"/>
       <c r="Y62" s="12"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:25" ht="15.75" customHeight="1">
       <c r="A63" s="12"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -2534,7 +2651,7 @@
       <c r="X63" s="12"/>
       <c r="Y63" s="12"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:25" ht="15.75" customHeight="1">
       <c r="A64" s="12"/>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
@@ -2561,7 +2678,7 @@
       <c r="X64" s="12"/>
       <c r="Y64" s="12"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:25" ht="15.75" customHeight="1">
       <c r="A65" s="12"/>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
@@ -2588,7 +2705,7 @@
       <c r="X65" s="12"/>
       <c r="Y65" s="12"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:25" ht="15.75" customHeight="1">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -2615,7 +2732,7 @@
       <c r="X66" s="12"/>
       <c r="Y66" s="12"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:25" ht="15.75" customHeight="1">
       <c r="A67" s="12"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
@@ -2642,7 +2759,7 @@
       <c r="X67" s="12"/>
       <c r="Y67" s="12"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:25" ht="15.75" customHeight="1">
       <c r="A68" s="12"/>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
@@ -2669,7 +2786,7 @@
       <c r="X68" s="12"/>
       <c r="Y68" s="12"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:25" ht="15.75" customHeight="1">
       <c r="A69" s="12"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
@@ -2696,7 +2813,7 @@
       <c r="X69" s="12"/>
       <c r="Y69" s="12"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:25" ht="15.75" customHeight="1">
       <c r="A70" s="12"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
@@ -2723,7 +2840,7 @@
       <c r="X70" s="12"/>
       <c r="Y70" s="12"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:25" ht="15.75" customHeight="1">
       <c r="A71" s="12"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
@@ -2750,7 +2867,7 @@
       <c r="X71" s="12"/>
       <c r="Y71" s="12"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:25" ht="15.75" customHeight="1">
       <c r="A72" s="12"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
@@ -2777,7 +2894,7 @@
       <c r="X72" s="12"/>
       <c r="Y72" s="12"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:25" ht="15.75" customHeight="1">
       <c r="A73" s="12"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
@@ -2804,7 +2921,7 @@
       <c r="X73" s="12"/>
       <c r="Y73" s="12"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:25" ht="15.75" customHeight="1">
       <c r="A74" s="12"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
@@ -2831,7 +2948,7 @@
       <c r="X74" s="12"/>
       <c r="Y74" s="12"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:25" ht="15.75" customHeight="1">
       <c r="A75" s="12"/>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
@@ -2858,7 +2975,7 @@
       <c r="X75" s="12"/>
       <c r="Y75" s="12"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" spans="1:25" ht="15.75" customHeight="1">
       <c r="A76" s="12"/>
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
@@ -2885,7 +3002,7 @@
       <c r="X76" s="12"/>
       <c r="Y76" s="12"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" spans="1:25" ht="15.75" customHeight="1">
       <c r="A77" s="12"/>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
@@ -2912,7 +3029,7 @@
       <c r="X77" s="12"/>
       <c r="Y77" s="12"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" spans="1:25" ht="15.75" customHeight="1">
       <c r="A78" s="12"/>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
@@ -2939,7 +3056,7 @@
       <c r="X78" s="12"/>
       <c r="Y78" s="12"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" spans="1:25" ht="15.75" customHeight="1">
       <c r="A79" s="12"/>
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
@@ -2966,7 +3083,7 @@
       <c r="X79" s="12"/>
       <c r="Y79" s="12"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" spans="1:25" ht="15.75" customHeight="1">
       <c r="A80" s="12"/>
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
@@ -2993,7 +3110,7 @@
       <c r="X80" s="12"/>
       <c r="Y80" s="12"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" spans="1:25" ht="15.75" customHeight="1">
       <c r="A81" s="12"/>
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
@@ -3020,7 +3137,7 @@
       <c r="X81" s="12"/>
       <c r="Y81" s="12"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" spans="1:25" ht="15.75" customHeight="1">
       <c r="A82" s="12"/>
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
@@ -3047,7 +3164,7 @@
       <c r="X82" s="12"/>
       <c r="Y82" s="12"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" spans="1:25" ht="15.75" customHeight="1">
       <c r="A83" s="12"/>
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
@@ -3074,7 +3191,7 @@
       <c r="X83" s="12"/>
       <c r="Y83" s="12"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" spans="1:25" ht="15.75" customHeight="1">
       <c r="A84" s="12"/>
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
@@ -3101,7 +3218,7 @@
       <c r="X84" s="12"/>
       <c r="Y84" s="12"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" spans="1:25" ht="15.75" customHeight="1">
       <c r="A85" s="12"/>
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
@@ -3128,7 +3245,7 @@
       <c r="X85" s="12"/>
       <c r="Y85" s="12"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" spans="1:25" ht="15.75" customHeight="1">
       <c r="A86" s="12"/>
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
@@ -3155,7 +3272,7 @@
       <c r="X86" s="12"/>
       <c r="Y86" s="12"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" spans="1:25" ht="15.75" customHeight="1">
       <c r="A87" s="12"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
@@ -3182,7 +3299,7 @@
       <c r="X87" s="12"/>
       <c r="Y87" s="12"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" spans="1:25" ht="15.75" customHeight="1">
       <c r="A88" s="12"/>
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
@@ -3209,7 +3326,7 @@
       <c r="X88" s="12"/>
       <c r="Y88" s="12"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" spans="1:25" ht="15.75" customHeight="1">
       <c r="A89" s="12"/>
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
@@ -3236,7 +3353,7 @@
       <c r="X89" s="12"/>
       <c r="Y89" s="12"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" spans="1:25" ht="15.75" customHeight="1">
       <c r="A90" s="12"/>
       <c r="B90" s="12"/>
       <c r="C90" s="12"/>
@@ -3263,7 +3380,7 @@
       <c r="X90" s="12"/>
       <c r="Y90" s="12"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" spans="1:25" ht="15.75" customHeight="1">
       <c r="A91" s="12"/>
       <c r="B91" s="12"/>
       <c r="C91" s="12"/>
@@ -3290,7 +3407,7 @@
       <c r="X91" s="12"/>
       <c r="Y91" s="12"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" spans="1:25" ht="15.75" customHeight="1">
       <c r="A92" s="12"/>
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
@@ -3317,7 +3434,7 @@
       <c r="X92" s="12"/>
       <c r="Y92" s="12"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" spans="1:25" ht="15.75" customHeight="1">
       <c r="A93" s="12"/>
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
@@ -3344,7 +3461,7 @@
       <c r="X93" s="12"/>
       <c r="Y93" s="12"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" spans="1:25" ht="15.75" customHeight="1">
       <c r="A94" s="12"/>
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
@@ -3371,7 +3488,7 @@
       <c r="X94" s="12"/>
       <c r="Y94" s="12"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" spans="1:25" ht="15.75" customHeight="1">
       <c r="A95" s="12"/>
       <c r="B95" s="12"/>
       <c r="C95" s="12"/>
@@ -3398,7 +3515,7 @@
       <c r="X95" s="12"/>
       <c r="Y95" s="12"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" spans="1:25" ht="15.75" customHeight="1">
       <c r="A96" s="12"/>
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
@@ -3425,7 +3542,7 @@
       <c r="X96" s="12"/>
       <c r="Y96" s="12"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" spans="1:25" ht="15.75" customHeight="1">
       <c r="A97" s="12"/>
       <c r="B97" s="12"/>
       <c r="C97" s="12"/>
@@ -3452,7 +3569,7 @@
       <c r="X97" s="12"/>
       <c r="Y97" s="12"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" spans="1:25" ht="15.75" customHeight="1">
       <c r="A98" s="12"/>
       <c r="B98" s="12"/>
       <c r="C98" s="12"/>
@@ -3479,7 +3596,7 @@
       <c r="X98" s="12"/>
       <c r="Y98" s="12"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" spans="1:25" ht="15.75" customHeight="1">
       <c r="A99" s="12"/>
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
@@ -3506,7 +3623,7 @@
       <c r="X99" s="12"/>
       <c r="Y99" s="12"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" spans="1:25" ht="15.75" customHeight="1">
       <c r="A100" s="12"/>
       <c r="B100" s="12"/>
       <c r="C100" s="12"/>
@@ -3533,7 +3650,7 @@
       <c r="X100" s="12"/>
       <c r="Y100" s="12"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" spans="1:25" ht="15.75" customHeight="1">
       <c r="A101" s="12"/>
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
@@ -3560,7 +3677,7 @@
       <c r="X101" s="12"/>
       <c r="Y101" s="12"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" spans="1:25" ht="15.75" customHeight="1">
       <c r="A102" s="12"/>
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
@@ -3587,7 +3704,7 @@
       <c r="X102" s="12"/>
       <c r="Y102" s="12"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" spans="1:25" ht="15.75" customHeight="1">
       <c r="A103" s="12"/>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
@@ -3614,7 +3731,7 @@
       <c r="X103" s="12"/>
       <c r="Y103" s="12"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" spans="1:25" ht="15.75" customHeight="1">
       <c r="A104" s="12"/>
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
@@ -3641,7 +3758,7 @@
       <c r="X104" s="12"/>
       <c r="Y104" s="12"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" spans="1:25" ht="15.75" customHeight="1">
       <c r="A105" s="12"/>
       <c r="B105" s="12"/>
       <c r="C105" s="12"/>
@@ -3668,7 +3785,7 @@
       <c r="X105" s="12"/>
       <c r="Y105" s="12"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" spans="1:25" ht="15.75" customHeight="1">
       <c r="A106" s="12"/>
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
@@ -3695,7 +3812,7 @@
       <c r="X106" s="12"/>
       <c r="Y106" s="12"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" spans="1:25" ht="15.75" customHeight="1">
       <c r="A107" s="12"/>
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
@@ -3722,7 +3839,7 @@
       <c r="X107" s="12"/>
       <c r="Y107" s="12"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" spans="1:25" ht="15.75" customHeight="1">
       <c r="A108" s="12"/>
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
@@ -3749,7 +3866,7 @@
       <c r="X108" s="12"/>
       <c r="Y108" s="12"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" spans="1:25" ht="15.75" customHeight="1">
       <c r="A109" s="12"/>
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
@@ -3776,7 +3893,7 @@
       <c r="X109" s="12"/>
       <c r="Y109" s="12"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" spans="1:25" ht="15.75" customHeight="1">
       <c r="A110" s="12"/>
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
@@ -3803,7 +3920,7 @@
       <c r="X110" s="12"/>
       <c r="Y110" s="12"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" spans="1:25" ht="15.75" customHeight="1">
       <c r="A111" s="12"/>
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
@@ -3830,7 +3947,7 @@
       <c r="X111" s="12"/>
       <c r="Y111" s="12"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" spans="1:25" ht="15.75" customHeight="1">
       <c r="A112" s="12"/>
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
@@ -3857,7 +3974,7 @@
       <c r="X112" s="12"/>
       <c r="Y112" s="12"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" spans="1:25" ht="15.75" customHeight="1">
       <c r="A113" s="12"/>
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
@@ -3884,7 +4001,7 @@
       <c r="X113" s="12"/>
       <c r="Y113" s="12"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" spans="1:25" ht="15.75" customHeight="1">
       <c r="A114" s="12"/>
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
@@ -3911,7 +4028,7 @@
       <c r="X114" s="12"/>
       <c r="Y114" s="12"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" spans="1:25" ht="15.75" customHeight="1">
       <c r="A115" s="12"/>
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
@@ -3938,7 +4055,7 @@
       <c r="X115" s="12"/>
       <c r="Y115" s="12"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" spans="1:25" ht="15.75" customHeight="1">
       <c r="A116" s="12"/>
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
@@ -3965,7 +4082,7 @@
       <c r="X116" s="12"/>
       <c r="Y116" s="12"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" spans="1:25" ht="15.75" customHeight="1">
       <c r="A117" s="12"/>
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
@@ -3992,7 +4109,7 @@
       <c r="X117" s="12"/>
       <c r="Y117" s="12"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" spans="1:25" ht="15.75" customHeight="1">
       <c r="A118" s="12"/>
       <c r="B118" s="12"/>
       <c r="C118" s="12"/>
@@ -4019,7 +4136,7 @@
       <c r="X118" s="12"/>
       <c r="Y118" s="12"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" spans="1:25" ht="15.75" customHeight="1">
       <c r="A119" s="12"/>
       <c r="B119" s="12"/>
       <c r="C119" s="12"/>
@@ -4046,7 +4163,7 @@
       <c r="X119" s="12"/>
       <c r="Y119" s="12"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" spans="1:25" ht="15.75" customHeight="1">
       <c r="A120" s="12"/>
       <c r="B120" s="12"/>
       <c r="C120" s="12"/>
@@ -4073,7 +4190,7 @@
       <c r="X120" s="12"/>
       <c r="Y120" s="12"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" spans="1:25" ht="15.75" customHeight="1">
       <c r="A121" s="12"/>
       <c r="B121" s="12"/>
       <c r="C121" s="12"/>
@@ -4100,7 +4217,7 @@
       <c r="X121" s="12"/>
       <c r="Y121" s="12"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" spans="1:25" ht="15.75" customHeight="1">
       <c r="A122" s="12"/>
       <c r="B122" s="12"/>
       <c r="C122" s="12"/>
@@ -4127,7 +4244,7 @@
       <c r="X122" s="12"/>
       <c r="Y122" s="12"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" spans="1:25" ht="15.75" customHeight="1">
       <c r="A123" s="12"/>
       <c r="B123" s="12"/>
       <c r="C123" s="12"/>
@@ -4154,7 +4271,7 @@
       <c r="X123" s="12"/>
       <c r="Y123" s="12"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" spans="1:25" ht="15.75" customHeight="1">
       <c r="A124" s="12"/>
       <c r="B124" s="12"/>
       <c r="C124" s="12"/>
@@ -4181,7 +4298,7 @@
       <c r="X124" s="12"/>
       <c r="Y124" s="12"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" spans="1:25" ht="15.75" customHeight="1">
       <c r="A125" s="12"/>
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
@@ -4208,7 +4325,7 @@
       <c r="X125" s="12"/>
       <c r="Y125" s="12"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" spans="1:25" ht="15.75" customHeight="1">
       <c r="A126" s="12"/>
       <c r="B126" s="12"/>
       <c r="C126" s="12"/>
@@ -4235,7 +4352,7 @@
       <c r="X126" s="12"/>
       <c r="Y126" s="12"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" spans="1:25" ht="15.75" customHeight="1">
       <c r="A127" s="12"/>
       <c r="B127" s="12"/>
       <c r="C127" s="12"/>
@@ -4262,7 +4379,7 @@
       <c r="X127" s="12"/>
       <c r="Y127" s="12"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" spans="1:25" ht="15.75" customHeight="1">
       <c r="A128" s="12"/>
       <c r="B128" s="12"/>
       <c r="C128" s="12"/>
@@ -4289,7 +4406,7 @@
       <c r="X128" s="12"/>
       <c r="Y128" s="12"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" spans="1:25" ht="15.75" customHeight="1">
       <c r="A129" s="12"/>
       <c r="B129" s="12"/>
       <c r="C129" s="12"/>
@@ -4316,7 +4433,7 @@
       <c r="X129" s="12"/>
       <c r="Y129" s="12"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" spans="1:25" ht="15.75" customHeight="1">
       <c r="A130" s="12"/>
       <c r="B130" s="12"/>
       <c r="C130" s="12"/>
@@ -4343,7 +4460,7 @@
       <c r="X130" s="12"/>
       <c r="Y130" s="12"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" spans="1:25" ht="15.75" customHeight="1">
       <c r="A131" s="12"/>
       <c r="B131" s="12"/>
       <c r="C131" s="12"/>
@@ -4370,7 +4487,7 @@
       <c r="X131" s="12"/>
       <c r="Y131" s="12"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" spans="1:25" ht="15.75" customHeight="1">
       <c r="A132" s="12"/>
       <c r="B132" s="12"/>
       <c r="C132" s="12"/>
@@ -4397,7 +4514,7 @@
       <c r="X132" s="12"/>
       <c r="Y132" s="12"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" spans="1:25" ht="15.75" customHeight="1">
       <c r="A133" s="12"/>
       <c r="B133" s="12"/>
       <c r="C133" s="12"/>
@@ -4424,7 +4541,7 @@
       <c r="X133" s="12"/>
       <c r="Y133" s="12"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" spans="1:25" ht="15.75" customHeight="1">
       <c r="A134" s="12"/>
       <c r="B134" s="12"/>
       <c r="C134" s="12"/>
@@ -4451,7 +4568,7 @@
       <c r="X134" s="12"/>
       <c r="Y134" s="12"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" spans="1:25" ht="15.75" customHeight="1">
       <c r="A135" s="12"/>
       <c r="B135" s="12"/>
       <c r="C135" s="12"/>
@@ -4478,7 +4595,7 @@
       <c r="X135" s="12"/>
       <c r="Y135" s="12"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" spans="1:25" ht="15.75" customHeight="1">
       <c r="A136" s="12"/>
       <c r="B136" s="12"/>
       <c r="C136" s="12"/>
@@ -4505,7 +4622,7 @@
       <c r="X136" s="12"/>
       <c r="Y136" s="12"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" spans="1:25" ht="15.75" customHeight="1">
       <c r="A137" s="12"/>
       <c r="B137" s="12"/>
       <c r="C137" s="12"/>
@@ -4532,7 +4649,7 @@
       <c r="X137" s="12"/>
       <c r="Y137" s="12"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" spans="1:25" ht="15.75" customHeight="1">
       <c r="A138" s="12"/>
       <c r="B138" s="12"/>
       <c r="C138" s="12"/>
@@ -4559,7 +4676,7 @@
       <c r="X138" s="12"/>
       <c r="Y138" s="12"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" spans="1:25" ht="15.75" customHeight="1">
       <c r="A139" s="12"/>
       <c r="B139" s="12"/>
       <c r="C139" s="12"/>
@@ -4586,7 +4703,7 @@
       <c r="X139" s="12"/>
       <c r="Y139" s="12"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" spans="1:25" ht="15.75" customHeight="1">
       <c r="A140" s="12"/>
       <c r="B140" s="12"/>
       <c r="C140" s="12"/>
@@ -4613,7 +4730,7 @@
       <c r="X140" s="12"/>
       <c r="Y140" s="12"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" spans="1:25" ht="15.75" customHeight="1">
       <c r="A141" s="12"/>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -4640,7 +4757,7 @@
       <c r="X141" s="12"/>
       <c r="Y141" s="12"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" spans="1:25" ht="15.75" customHeight="1">
       <c r="A142" s="12"/>
       <c r="B142" s="12"/>
       <c r="C142" s="12"/>
@@ -4667,7 +4784,7 @@
       <c r="X142" s="12"/>
       <c r="Y142" s="12"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" spans="1:25" ht="15.75" customHeight="1">
       <c r="A143" s="12"/>
       <c r="B143" s="12"/>
       <c r="C143" s="12"/>
@@ -4694,7 +4811,7 @@
       <c r="X143" s="12"/>
       <c r="Y143" s="12"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" spans="1:25" ht="15.75" customHeight="1">
       <c r="A144" s="12"/>
       <c r="B144" s="12"/>
       <c r="C144" s="12"/>
@@ -4721,7 +4838,7 @@
       <c r="X144" s="12"/>
       <c r="Y144" s="12"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" spans="1:25" ht="15.75" customHeight="1">
       <c r="A145" s="12"/>
       <c r="B145" s="12"/>
       <c r="C145" s="12"/>
@@ -4748,7 +4865,7 @@
       <c r="X145" s="12"/>
       <c r="Y145" s="12"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" spans="1:25" ht="15.75" customHeight="1">
       <c r="A146" s="12"/>
       <c r="B146" s="12"/>
       <c r="C146" s="12"/>
@@ -4775,7 +4892,7 @@
       <c r="X146" s="12"/>
       <c r="Y146" s="12"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" spans="1:25" ht="15.75" customHeight="1">
       <c r="A147" s="12"/>
       <c r="B147" s="12"/>
       <c r="C147" s="12"/>
@@ -4802,7 +4919,7 @@
       <c r="X147" s="12"/>
       <c r="Y147" s="12"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" spans="1:25" ht="15.75" customHeight="1">
       <c r="A148" s="12"/>
       <c r="B148" s="12"/>
       <c r="C148" s="12"/>
@@ -4829,7 +4946,7 @@
       <c r="X148" s="12"/>
       <c r="Y148" s="12"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" spans="1:25" ht="15.75" customHeight="1">
       <c r="A149" s="12"/>
       <c r="B149" s="12"/>
       <c r="C149" s="12"/>
@@ -4856,7 +4973,7 @@
       <c r="X149" s="12"/>
       <c r="Y149" s="12"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" spans="1:25" ht="15.75" customHeight="1">
       <c r="A150" s="12"/>
       <c r="B150" s="12"/>
       <c r="C150" s="12"/>
@@ -4883,7 +5000,7 @@
       <c r="X150" s="12"/>
       <c r="Y150" s="12"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" spans="1:25" ht="15.75" customHeight="1">
       <c r="A151" s="12"/>
       <c r="B151" s="12"/>
       <c r="C151" s="12"/>
@@ -4910,7 +5027,7 @@
       <c r="X151" s="12"/>
       <c r="Y151" s="12"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" spans="1:25" ht="15.75" customHeight="1">
       <c r="A152" s="12"/>
       <c r="B152" s="12"/>
       <c r="C152" s="12"/>
@@ -4937,7 +5054,7 @@
       <c r="X152" s="12"/>
       <c r="Y152" s="12"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" spans="1:25" ht="15.75" customHeight="1">
       <c r="A153" s="12"/>
       <c r="B153" s="12"/>
       <c r="C153" s="12"/>
@@ -4964,7 +5081,7 @@
       <c r="X153" s="12"/>
       <c r="Y153" s="12"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" spans="1:25" ht="15.75" customHeight="1">
       <c r="A154" s="12"/>
       <c r="B154" s="12"/>
       <c r="C154" s="12"/>
@@ -4991,7 +5108,7 @@
       <c r="X154" s="12"/>
       <c r="Y154" s="12"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" spans="1:25" ht="15.75" customHeight="1">
       <c r="A155" s="12"/>
       <c r="B155" s="12"/>
       <c r="C155" s="12"/>
@@ -5018,7 +5135,7 @@
       <c r="X155" s="12"/>
       <c r="Y155" s="12"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" spans="1:25" ht="15.75" customHeight="1">
       <c r="A156" s="12"/>
       <c r="B156" s="12"/>
       <c r="C156" s="12"/>
@@ -5045,7 +5162,7 @@
       <c r="X156" s="12"/>
       <c r="Y156" s="12"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" spans="1:25" ht="15.75" customHeight="1">
       <c r="A157" s="12"/>
       <c r="B157" s="12"/>
       <c r="C157" s="12"/>
@@ -5072,7 +5189,7 @@
       <c r="X157" s="12"/>
       <c r="Y157" s="12"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" spans="1:25" ht="15.75" customHeight="1">
       <c r="A158" s="12"/>
       <c r="B158" s="12"/>
       <c r="C158" s="12"/>
@@ -5099,7 +5216,7 @@
       <c r="X158" s="12"/>
       <c r="Y158" s="12"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" spans="1:25" ht="15.75" customHeight="1">
       <c r="A159" s="12"/>
       <c r="B159" s="12"/>
       <c r="C159" s="12"/>
@@ -5126,7 +5243,7 @@
       <c r="X159" s="12"/>
       <c r="Y159" s="12"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" spans="1:25" ht="15.75" customHeight="1">
       <c r="A160" s="12"/>
       <c r="B160" s="12"/>
       <c r="C160" s="12"/>
@@ -5153,7 +5270,7 @@
       <c r="X160" s="12"/>
       <c r="Y160" s="12"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" spans="1:25" ht="15.75" customHeight="1">
       <c r="A161" s="12"/>
       <c r="B161" s="12"/>
       <c r="C161" s="12"/>
@@ -5180,7 +5297,7 @@
       <c r="X161" s="12"/>
       <c r="Y161" s="12"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" spans="1:25" ht="15.75" customHeight="1">
       <c r="A162" s="12"/>
       <c r="B162" s="12"/>
       <c r="C162" s="12"/>
@@ -5207,7 +5324,7 @@
       <c r="X162" s="12"/>
       <c r="Y162" s="12"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" spans="1:25" ht="15.75" customHeight="1">
       <c r="A163" s="12"/>
       <c r="B163" s="12"/>
       <c r="C163" s="12"/>
@@ -5234,7 +5351,7 @@
       <c r="X163" s="12"/>
       <c r="Y163" s="12"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" spans="1:25" ht="15.75" customHeight="1">
       <c r="A164" s="12"/>
       <c r="B164" s="12"/>
       <c r="C164" s="12"/>
@@ -5261,7 +5378,7 @@
       <c r="X164" s="12"/>
       <c r="Y164" s="12"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" spans="1:25" ht="15.75" customHeight="1">
       <c r="A165" s="12"/>
       <c r="B165" s="12"/>
       <c r="C165" s="12"/>
@@ -5288,7 +5405,7 @@
       <c r="X165" s="12"/>
       <c r="Y165" s="12"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" spans="1:25" ht="15.75" customHeight="1">
       <c r="A166" s="12"/>
       <c r="B166" s="12"/>
       <c r="C166" s="12"/>
@@ -5315,7 +5432,7 @@
       <c r="X166" s="12"/>
       <c r="Y166" s="12"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" spans="1:25" ht="15.75" customHeight="1">
       <c r="A167" s="12"/>
       <c r="B167" s="12"/>
       <c r="C167" s="12"/>
@@ -5342,7 +5459,7 @@
       <c r="X167" s="12"/>
       <c r="Y167" s="12"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" spans="1:25" ht="15.75" customHeight="1">
       <c r="A168" s="12"/>
       <c r="B168" s="12"/>
       <c r="C168" s="12"/>
@@ -5369,7 +5486,7 @@
       <c r="X168" s="12"/>
       <c r="Y168" s="12"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" spans="1:25" ht="15.75" customHeight="1">
       <c r="A169" s="12"/>
       <c r="B169" s="12"/>
       <c r="C169" s="12"/>
@@ -5396,7 +5513,7 @@
       <c r="X169" s="12"/>
       <c r="Y169" s="12"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" spans="1:25" ht="15.75" customHeight="1">
       <c r="A170" s="12"/>
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
@@ -5423,7 +5540,7 @@
       <c r="X170" s="12"/>
       <c r="Y170" s="12"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" spans="1:25" ht="15.75" customHeight="1">
       <c r="A171" s="12"/>
       <c r="B171" s="12"/>
       <c r="C171" s="12"/>
@@ -5450,7 +5567,7 @@
       <c r="X171" s="12"/>
       <c r="Y171" s="12"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" spans="1:25" ht="15.75" customHeight="1">
       <c r="A172" s="12"/>
       <c r="B172" s="12"/>
       <c r="C172" s="12"/>
@@ -5477,7 +5594,7 @@
       <c r="X172" s="12"/>
       <c r="Y172" s="12"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" spans="1:25" ht="15.75" customHeight="1">
       <c r="A173" s="12"/>
       <c r="B173" s="12"/>
       <c r="C173" s="12"/>
@@ -5504,7 +5621,7 @@
       <c r="X173" s="12"/>
       <c r="Y173" s="12"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" spans="1:25" ht="15.75" customHeight="1">
       <c r="A174" s="12"/>
       <c r="B174" s="12"/>
       <c r="C174" s="12"/>
@@ -5531,7 +5648,7 @@
       <c r="X174" s="12"/>
       <c r="Y174" s="12"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" spans="1:25" ht="15.75" customHeight="1">
       <c r="A175" s="12"/>
       <c r="B175" s="12"/>
       <c r="C175" s="12"/>
@@ -5558,7 +5675,7 @@
       <c r="X175" s="12"/>
       <c r="Y175" s="12"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" spans="1:25" ht="15.75" customHeight="1">
       <c r="A176" s="12"/>
       <c r="B176" s="12"/>
       <c r="C176" s="12"/>
@@ -5585,7 +5702,7 @@
       <c r="X176" s="12"/>
       <c r="Y176" s="12"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" spans="1:25" ht="15.75" customHeight="1">
       <c r="A177" s="12"/>
       <c r="B177" s="12"/>
       <c r="C177" s="12"/>
@@ -5612,7 +5729,7 @@
       <c r="X177" s="12"/>
       <c r="Y177" s="12"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" spans="1:25" ht="15.75" customHeight="1">
       <c r="A178" s="12"/>
       <c r="B178" s="12"/>
       <c r="C178" s="12"/>
@@ -5639,7 +5756,7 @@
       <c r="X178" s="12"/>
       <c r="Y178" s="12"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" spans="1:25" ht="15.75" customHeight="1">
       <c r="A179" s="12"/>
       <c r="B179" s="12"/>
       <c r="C179" s="12"/>
@@ -5666,7 +5783,7 @@
       <c r="X179" s="12"/>
       <c r="Y179" s="12"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" spans="1:25" ht="15.75" customHeight="1">
       <c r="A180" s="12"/>
       <c r="B180" s="12"/>
       <c r="C180" s="12"/>
@@ -5693,7 +5810,7 @@
       <c r="X180" s="12"/>
       <c r="Y180" s="12"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" spans="1:25" ht="15.75" customHeight="1">
       <c r="A181" s="12"/>
       <c r="B181" s="12"/>
       <c r="C181" s="12"/>
@@ -5720,7 +5837,7 @@
       <c r="X181" s="12"/>
       <c r="Y181" s="12"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" spans="1:25" ht="15.75" customHeight="1">
       <c r="A182" s="12"/>
       <c r="B182" s="12"/>
       <c r="C182" s="12"/>
@@ -5747,7 +5864,7 @@
       <c r="X182" s="12"/>
       <c r="Y182" s="12"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" spans="1:25" ht="15.75" customHeight="1">
       <c r="A183" s="12"/>
       <c r="B183" s="12"/>
       <c r="C183" s="12"/>
@@ -5774,7 +5891,7 @@
       <c r="X183" s="12"/>
       <c r="Y183" s="12"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" spans="1:25" ht="15.75" customHeight="1">
       <c r="A184" s="12"/>
       <c r="B184" s="12"/>
       <c r="C184" s="12"/>
@@ -5801,7 +5918,7 @@
       <c r="X184" s="12"/>
       <c r="Y184" s="12"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" spans="1:25" ht="15.75" customHeight="1">
       <c r="A185" s="12"/>
       <c r="B185" s="12"/>
       <c r="C185" s="12"/>
@@ -5828,7 +5945,7 @@
       <c r="X185" s="12"/>
       <c r="Y185" s="12"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" spans="1:25" ht="15.75" customHeight="1">
       <c r="A186" s="12"/>
       <c r="B186" s="12"/>
       <c r="C186" s="12"/>
@@ -5855,7 +5972,7 @@
       <c r="X186" s="12"/>
       <c r="Y186" s="12"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" spans="1:25" ht="15.75" customHeight="1">
       <c r="A187" s="12"/>
       <c r="B187" s="12"/>
       <c r="C187" s="12"/>
@@ -5882,7 +5999,7 @@
       <c r="X187" s="12"/>
       <c r="Y187" s="12"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" spans="1:25" ht="15.75" customHeight="1">
       <c r="A188" s="12"/>
       <c r="B188" s="12"/>
       <c r="C188" s="12"/>
@@ -5909,7 +6026,7 @@
       <c r="X188" s="12"/>
       <c r="Y188" s="12"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" spans="1:25" ht="15.75" customHeight="1">
       <c r="A189" s="12"/>
       <c r="B189" s="12"/>
       <c r="C189" s="12"/>
@@ -5936,7 +6053,7 @@
       <c r="X189" s="12"/>
       <c r="Y189" s="12"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" spans="1:25" ht="15.75" customHeight="1">
       <c r="A190" s="12"/>
       <c r="B190" s="12"/>
       <c r="C190" s="12"/>
@@ -5963,7 +6080,7 @@
       <c r="X190" s="12"/>
       <c r="Y190" s="12"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" spans="1:25" ht="15.75" customHeight="1">
       <c r="A191" s="12"/>
       <c r="B191" s="12"/>
       <c r="C191" s="12"/>
@@ -5990,7 +6107,7 @@
       <c r="X191" s="12"/>
       <c r="Y191" s="12"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" spans="1:25" ht="15.75" customHeight="1">
       <c r="A192" s="12"/>
       <c r="B192" s="12"/>
       <c r="C192" s="12"/>
@@ -6017,7 +6134,7 @@
       <c r="X192" s="12"/>
       <c r="Y192" s="12"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" spans="1:25" ht="15.75" customHeight="1">
       <c r="A193" s="12"/>
       <c r="B193" s="12"/>
       <c r="C193" s="12"/>
@@ -6044,7 +6161,7 @@
       <c r="X193" s="12"/>
       <c r="Y193" s="12"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" spans="1:25" ht="15.75" customHeight="1">
       <c r="A194" s="12"/>
       <c r="B194" s="12"/>
       <c r="C194" s="12"/>
@@ -6071,7 +6188,7 @@
       <c r="X194" s="12"/>
       <c r="Y194" s="12"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" spans="1:25" ht="15.75" customHeight="1">
       <c r="A195" s="12"/>
       <c r="B195" s="12"/>
       <c r="C195" s="12"/>
@@ -6098,7 +6215,7 @@
       <c r="X195" s="12"/>
       <c r="Y195" s="12"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" spans="1:25" ht="15.75" customHeight="1">
       <c r="A196" s="12"/>
       <c r="B196" s="12"/>
       <c r="C196" s="12"/>
@@ -6125,7 +6242,7 @@
       <c r="X196" s="12"/>
       <c r="Y196" s="12"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" spans="1:25" ht="15.75" customHeight="1">
       <c r="A197" s="12"/>
       <c r="B197" s="12"/>
       <c r="C197" s="12"/>
@@ -6152,7 +6269,7 @@
       <c r="X197" s="12"/>
       <c r="Y197" s="12"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" spans="1:25" ht="15.75" customHeight="1">
       <c r="A198" s="12"/>
       <c r="B198" s="12"/>
       <c r="C198" s="12"/>
@@ -6179,7 +6296,7 @@
       <c r="X198" s="12"/>
       <c r="Y198" s="12"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" spans="1:25" ht="15.75" customHeight="1">
       <c r="A199" s="12"/>
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
@@ -6206,7 +6323,7 @@
       <c r="X199" s="12"/>
       <c r="Y199" s="12"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="1:25" ht="15.75" customHeight="1">
       <c r="A200" s="12"/>
       <c r="B200" s="12"/>
       <c r="C200" s="12"/>
@@ -6233,7 +6350,7 @@
       <c r="X200" s="12"/>
       <c r="Y200" s="12"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="1:25" ht="15.75" customHeight="1">
       <c r="A201" s="12"/>
       <c r="B201" s="12"/>
       <c r="C201" s="12"/>
@@ -6260,7 +6377,7 @@
       <c r="X201" s="12"/>
       <c r="Y201" s="12"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="1:25" ht="15.75" customHeight="1">
       <c r="A202" s="12"/>
       <c r="B202" s="12"/>
       <c r="C202" s="12"/>
@@ -6287,7 +6404,7 @@
       <c r="X202" s="12"/>
       <c r="Y202" s="12"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" spans="1:25" ht="15.75" customHeight="1">
       <c r="A203" s="12"/>
       <c r="B203" s="12"/>
       <c r="C203" s="12"/>
@@ -6314,7 +6431,7 @@
       <c r="X203" s="12"/>
       <c r="Y203" s="12"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="1:25" ht="15.75" customHeight="1">
       <c r="A204" s="12"/>
       <c r="B204" s="12"/>
       <c r="C204" s="12"/>
@@ -6341,7 +6458,7 @@
       <c r="X204" s="12"/>
       <c r="Y204" s="12"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" spans="1:25" ht="15.75" customHeight="1">
       <c r="A205" s="12"/>
       <c r="B205" s="12"/>
       <c r="C205" s="12"/>
@@ -6368,7 +6485,7 @@
       <c r="X205" s="12"/>
       <c r="Y205" s="12"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="1:25" ht="15.75" customHeight="1">
       <c r="A206" s="12"/>
       <c r="B206" s="12"/>
       <c r="C206" s="12"/>
@@ -6395,7 +6512,7 @@
       <c r="X206" s="12"/>
       <c r="Y206" s="12"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="1:25" ht="15.75" customHeight="1">
       <c r="A207" s="12"/>
       <c r="B207" s="12"/>
       <c r="C207" s="12"/>
@@ -6422,7 +6539,7 @@
       <c r="X207" s="12"/>
       <c r="Y207" s="12"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" spans="1:25" ht="15.75" customHeight="1">
       <c r="A208" s="12"/>
       <c r="B208" s="12"/>
       <c r="C208" s="12"/>
@@ -6449,7 +6566,7 @@
       <c r="X208" s="12"/>
       <c r="Y208" s="12"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" spans="1:25" ht="15.75" customHeight="1">
       <c r="A209" s="12"/>
       <c r="B209" s="12"/>
       <c r="C209" s="12"/>
@@ -6476,7 +6593,7 @@
       <c r="X209" s="12"/>
       <c r="Y209" s="12"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="1:25" ht="15.75" customHeight="1">
       <c r="A210" s="12"/>
       <c r="B210" s="12"/>
       <c r="C210" s="12"/>
@@ -6503,7 +6620,7 @@
       <c r="X210" s="12"/>
       <c r="Y210" s="12"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" spans="1:25" ht="15.75" customHeight="1">
       <c r="A211" s="12"/>
       <c r="B211" s="12"/>
       <c r="C211" s="12"/>
@@ -6530,7 +6647,7 @@
       <c r="X211" s="12"/>
       <c r="Y211" s="12"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" spans="1:25" ht="15.75" customHeight="1">
       <c r="A212" s="12"/>
       <c r="B212" s="12"/>
       <c r="C212" s="12"/>
@@ -6557,7 +6674,7 @@
       <c r="X212" s="12"/>
       <c r="Y212" s="12"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="1:25" ht="15.75" customHeight="1">
       <c r="A213" s="12"/>
       <c r="B213" s="12"/>
       <c r="C213" s="12"/>
@@ -6584,7 +6701,7 @@
       <c r="X213" s="12"/>
       <c r="Y213" s="12"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="1:25" ht="15.75" customHeight="1">
       <c r="A214" s="12"/>
       <c r="B214" s="12"/>
       <c r="C214" s="12"/>
@@ -6611,7 +6728,7 @@
       <c r="X214" s="12"/>
       <c r="Y214" s="12"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="1:25" ht="15.75" customHeight="1">
       <c r="A215" s="12"/>
       <c r="B215" s="12"/>
       <c r="C215" s="12"/>
@@ -6638,7 +6755,7 @@
       <c r="X215" s="12"/>
       <c r="Y215" s="12"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" spans="1:25" ht="15.75" customHeight="1">
       <c r="A216" s="12"/>
       <c r="B216" s="12"/>
       <c r="C216" s="12"/>
@@ -6665,7 +6782,7 @@
       <c r="X216" s="12"/>
       <c r="Y216" s="12"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" spans="1:25" ht="15.75" customHeight="1">
       <c r="A217" s="12"/>
       <c r="B217" s="12"/>
       <c r="C217" s="12"/>
@@ -6692,7 +6809,7 @@
       <c r="X217" s="12"/>
       <c r="Y217" s="12"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" spans="1:25" ht="15.75" customHeight="1">
       <c r="A218" s="12"/>
       <c r="B218" s="12"/>
       <c r="C218" s="12"/>
@@ -6719,7 +6836,7 @@
       <c r="X218" s="12"/>
       <c r="Y218" s="12"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="1:25" ht="15.75" customHeight="1">
       <c r="A219" s="12"/>
       <c r="B219" s="12"/>
       <c r="C219" s="12"/>
@@ -6746,7 +6863,7 @@
       <c r="X219" s="12"/>
       <c r="Y219" s="12"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" spans="1:25" ht="15.75" customHeight="1">
       <c r="A220" s="12"/>
       <c r="B220" s="12"/>
       <c r="C220" s="12"/>
@@ -7554,90 +7671,93 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.13"/>
-    <col customWidth="1" min="5" max="5" width="31.38"/>
+    <col min="2" max="2" customWidth="true" width="21.142857142857142"/>
+    <col min="5" max="5" customWidth="true" width="31.428571428571427"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>39</v>
+      <c r="B1" s="16" t="s">
+        <v>33</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>13</v>
+      <c r="C1" s="16" t="s">
+        <v>9</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>40</v>
+      <c r="D1" s="16" t="s">
+        <v>34</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>41</v>
+      <c r="E1" s="16" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2">
-      <formula1>"1,2"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" ht="15">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{a8934887-2acd-469b-8ed5-533fbe88b3c4}">
+  <dimension ref="A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="5" spans="1:1" ht="23.25" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update tc game file jar
</commit_message>
<xml_diff>
--- a/config/Scope.xlsx
+++ b/config/Scope.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Options" sheetId="3" r:id="rId5"/>
     <sheet name="Group-Turn" sheetId="4" r:id="rId6"/>
     <sheet name="Note" sheetId="5" r:id="rId7"/>
-    <sheet name="Evaluation Warning" sheetId="22" r:id="rId8"/>
+    <sheet name="Evaluation Warning" sheetId="27" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -149,7 +149,7 @@
     <t>Evaluation Only. Created with Aspose.Cells for Java.Copyright 2003 - 2021 Aspose Pty Ltd.</t>
   </si>
   <si>
-    <t>Report_BE.RS02WordMachine(Clone)</t>
+    <t>Report_BE.IP02(Clone)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +288,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,50 +315,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
@@ -683,12 +639,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y19"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
@@ -1229,8 +1185,143 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
     </row>
+    <row r="20" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D19">
+  <conditionalFormatting sqref="D1:D24">
     <cfRule type="cellIs" priority="1" dxfId="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
@@ -1242,7 +1333,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E19">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E24">
       <formula1>'Group-Turn'!$A:$A</formula1>
     </dataValidation>
   </dataValidations>
@@ -1259,7 +1350,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="topLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
@@ -1319,7 +1410,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D2" s="11">
         <v>1.0</v>
@@ -9190,7 +9281,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{daf57138-c2d7-43f1-869d-965a519aefb2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{c5aaf85d-571b-4cc3-be0a-5ce6ba3a55e5}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
@@ -9198,7 +9289,7 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="5" spans="1:1" ht="23.25" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="19" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>